<commit_message>
Spreadsheet importer custom attribute tests Added a default context to location problems which do not have a parent
</commit_message>
<xml_diff>
--- a/georegistry-test/src/test/resources/test-spreadsheet.xlsx
+++ b/georegistry-test/src/test/resources/test-spreadsheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
   <si>
     <t xml:space="preserve">Longitude</t>
   </si>
@@ -40,6 +40,18 @@
     <t xml:space="preserve">Term</t>
   </si>
   <si>
+    <t xml:space="preserve">Test Integer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Boolean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test Float</t>
+  </si>
+  <si>
     <t xml:space="preserve">Test</t>
   </si>
   <si>
@@ -47,14 +59,19 @@
   </si>
   <si>
     <t xml:space="preserve">Test Term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Empty</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="166" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -121,8 +138,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -143,10 +168,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P24" activeCellId="0" sqref="P24"/>
+      <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -173,6 +198,18 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -182,17 +219,45 @@
         <v>2.232343</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>8</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>43143</v>
+      </c>
+      <c r="I2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="J2" s="0" t="n">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>1.134232</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>2.232343</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>